<commit_message>
change 9_test print, change to only window size 15 for testing
</commit_message>
<xml_diff>
--- a/window_test/80_20_test.xlsx
+++ b/window_test/80_20_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\basill\research\steps\window_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BF0834FA-7FAE-48E9-AF75-3978C1362D42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2DE5074E-32DA-46DF-9A43-314719C479B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16590" yWindow="3330" windowWidth="19200" windowHeight="11505"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="80_20_test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2762" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2781" uniqueCount="30">
   <si>
     <t>Window size</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Ankle</t>
+  </si>
+  <si>
+    <t>Averaged ALL</t>
+  </si>
+  <si>
+    <t>1 second window</t>
   </si>
 </sst>
 </file>
@@ -451,7 +457,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -573,6 +579,19 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -749,6 +768,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -794,7 +826,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -807,24 +839,21 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -833,14 +862,23 @@
     <xf numFmtId="0" fontId="16" fillId="35" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1199,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2701"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="W26" sqref="W26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,8 +1597,10 @@
       <c r="K8">
         <v>0.987341772151898</v>
       </c>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+      <c r="M8" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="22"/>
       <c r="O8" s="4" t="s">
         <v>18</v>
       </c>
@@ -2492,6 +2532,18 @@
       <c r="K22">
         <v>0.192393736017897</v>
       </c>
+      <c r="M22" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="N22" s="22"/>
+      <c r="O22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R22" s="4"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -2527,6 +2579,24 @@
       <c r="K23">
         <v>0.95486935866983302</v>
       </c>
+      <c r="M23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -2562,6 +2632,28 @@
       <c r="K24">
         <v>0.84136967155834996</v>
       </c>
+      <c r="M24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N24" s="3">
+        <v>1</v>
+      </c>
+      <c r="O24" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "regular", $D$2:$D$271, "1" )</f>
+        <v>1.0055375000000002</v>
+      </c>
+      <c r="P24" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "regular", $D$2:$D$271, "1" )</f>
+        <v>0.97148940351255098</v>
+      </c>
+      <c r="Q24" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "regular", $D$2:$D$271, "1" )</f>
+        <v>1.0163</v>
+      </c>
+      <c r="R24" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "regular", $D$2:$D$271, "1" )</f>
+        <v>0.95688077292477891</v>
+      </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -2597,6 +2689,28 @@
       <c r="K25">
         <v>0.165548098434004</v>
       </c>
+      <c r="M25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N25" s="3">
+        <v>2</v>
+      </c>
+      <c r="O25" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "regular", $D$2:$D$271, "2" )</f>
+        <v>0.98962500000000009</v>
+      </c>
+      <c r="P25" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "regular", $D$2:$D$271, "2" )</f>
+        <v>0.97506948012306693</v>
+      </c>
+      <c r="Q25" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "regular", $D$2:$D$271, "2" )</f>
+        <v>0.97856666666666658</v>
+      </c>
+      <c r="R25" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "regular", $D$2:$D$271, "2" )</f>
+        <v>0.97100901429159536</v>
+      </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -2632,6 +2746,28 @@
       <c r="K26">
         <v>0.95346628679961998</v>
       </c>
+      <c r="M26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N26" s="3">
+        <v>3</v>
+      </c>
+      <c r="O26" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "regular", $D$2:$D$271, "3" )</f>
+        <v>0.98687083333333325</v>
+      </c>
+      <c r="P26" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "regular", $D$2:$D$271, "3" )</f>
+        <v>0.97481851464333291</v>
+      </c>
+      <c r="Q26" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "regular", $D$2:$D$271, "3" )</f>
+        <v>0.98641666666666683</v>
+      </c>
+      <c r="R26" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "regular", $D$2:$D$271, "3" )</f>
+        <v>0.9489156862828364</v>
+      </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -2667,6 +2803,28 @@
       <c r="K27">
         <v>0.93860845839017704</v>
       </c>
+      <c r="M27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N27" s="3">
+        <v>1</v>
+      </c>
+      <c r="O27" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "semiregular", $D$2:$D$271, "1" )</f>
+        <v>0.99611250000000007</v>
+      </c>
+      <c r="P27" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "semiregular", $D$2:$D$271, "1" )</f>
+        <v>0.8027695208487976</v>
+      </c>
+      <c r="Q27" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "semiregular", $D$2:$D$271, "1" )</f>
+        <v>0.99734999999999996</v>
+      </c>
+      <c r="R27" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "semiregular", $D$2:$D$271, "1" )</f>
+        <v>0.81775489631484666</v>
+      </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -2702,6 +2860,28 @@
       <c r="K28">
         <v>0.88143176733780704</v>
       </c>
+      <c r="M28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N28" s="3">
+        <v>2</v>
+      </c>
+      <c r="O28" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "semiregular", $D$2:$D$271, "2" )</f>
+        <v>0.99391250000000009</v>
+      </c>
+      <c r="P28" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "semiregular", $D$2:$D$271, "2" )</f>
+        <v>0.82428239640237433</v>
+      </c>
+      <c r="Q28" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "semiregular", $D$2:$D$271, "2" )</f>
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="R28" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "semiregular", $D$2:$D$271, "2" )</f>
+        <v>0.81931193955895132</v>
+      </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -2737,6 +2917,28 @@
       <c r="K29">
         <v>0.98137210358927696</v>
       </c>
+      <c r="M29" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N29" s="3">
+        <v>3</v>
+      </c>
+      <c r="O29" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "semiregular", $D$2:$D$271, "3" )</f>
+        <v>1.0123666666666669</v>
+      </c>
+      <c r="P29" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "semiregular", $D$2:$D$271, "3" )</f>
+        <v>0.91081243302883863</v>
+      </c>
+      <c r="Q29" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "semiregular", $D$2:$D$271, "3" )</f>
+        <v>1.0030166666666667</v>
+      </c>
+      <c r="R29" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "semiregular", $D$2:$D$271, "3" )</f>
+        <v>0.90587551013517775</v>
+      </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -2772,6 +2974,28 @@
       <c r="K30">
         <v>0.78228782287822896</v>
       </c>
+      <c r="M30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="3">
+        <v>1</v>
+      </c>
+      <c r="O30" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "irregular", $D$2:$D$271, "1" )</f>
+        <v>1.0186833333333334</v>
+      </c>
+      <c r="P30" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "irregular", $D$2:$D$271, "1" )</f>
+        <v>0.18423803241966197</v>
+      </c>
+      <c r="Q30" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "irregular", $D$2:$D$271, "1" )</f>
+        <v>1.3985666666666665</v>
+      </c>
+      <c r="R30" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "irregular", $D$2:$D$271, "1" )</f>
+        <v>0.15776364231787895</v>
+      </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -2807,6 +3031,28 @@
       <c r="K31">
         <v>0.18181818181818099</v>
       </c>
+      <c r="M31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" s="3">
+        <v>2</v>
+      </c>
+      <c r="O31" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "irregular", $D$2:$D$271, "2" )</f>
+        <v>0.98541249999999991</v>
+      </c>
+      <c r="P31" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "irregular", $D$2:$D$271, "2" )</f>
+        <v>0.19283327939316422</v>
+      </c>
+      <c r="Q31" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "irregular", $D$2:$D$271, "2" )</f>
+        <v>1.31595</v>
+      </c>
+      <c r="R31" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "irregular", $D$2:$D$271, "2" )</f>
+        <v>0.15405858991835267</v>
+      </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -2842,6 +3088,28 @@
       <c r="K32">
         <v>0.97909090909090901</v>
       </c>
+      <c r="M32" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N32" s="3">
+        <v>3</v>
+      </c>
+      <c r="O32" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "irregular", $D$2:$D$271, "3" )</f>
+        <v>0.96284999999999987</v>
+      </c>
+      <c r="P32" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&lt;25", $C$2:$C$271, "irregular", $D$2:$D$271, "3" )</f>
+        <v>0.83420239094935378</v>
+      </c>
+      <c r="Q32" s="8">
+        <f>AVERAGEIFS($J$2:$J$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "irregular", $D$2:$D$271, "3" )</f>
+        <v>1.0324333333333333</v>
+      </c>
+      <c r="R32" s="8">
+        <f>AVERAGEIFS($K$2:$K$271, $B$2:$B$271, "&gt;=25", $C$2:$C$271, "irregular", $D$2:$D$271, "3" )</f>
+        <v>0.78452732830325844</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
@@ -96259,9 +96527,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
     <mergeCell ref="T7:Z7"/>
     <mergeCell ref="T14:Z14"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M22:N22"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="Q8:R8"/>
     <mergeCell ref="U8:V8"/>

</xml_diff>